<commit_message>
Atualizado por script em 04-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/china_super-league_2023.xlsx
+++ b/2023/china_super-league_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V233"/>
+  <dimension ref="A1:V240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1125,71 +1125,71 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Shanghai Shenhua</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Qingdao Hainiu</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Shandong Taishan</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
       <c r="J8" t="n">
-        <v>3.88</v>
+        <v>5.38</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>14/04/2023 13:16</t>
+          <t>15/04/2023 16:18</t>
         </is>
       </c>
       <c r="L8" t="n">
-        <v>3.16</v>
+        <v>7.05</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>16/04/2023 13:30</t>
+          <t>16/04/2023 13:34</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>3.42</v>
+        <v>3.66</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>14/04/2023 13:16</t>
+          <t>15/04/2023 16:18</t>
         </is>
       </c>
       <c r="P8" t="n">
-        <v>3.31</v>
+        <v>4.04</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>16/04/2023 13:27</t>
+          <t>16/04/2023 13:34</t>
         </is>
       </c>
       <c r="R8" t="n">
-        <v>1.98</v>
+        <v>1.67</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>14/04/2023 13:16</t>
+          <t>15/04/2023 16:18</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>2.35</v>
+        <v>1.51</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>16/04/2023 13:30</t>
+          <t>16/04/2023 13:34</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/shanghai-shenhua-shandong-taishan/4O7XHmWo/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/shenzhen-fc-qingdao-hainiu/YcCyH7oh/</t>
         </is>
       </c>
     </row>
@@ -1217,71 +1217,71 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Shenzhen</t>
+          <t>Shanghai Shenhua</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Qingdao Hainiu</t>
+          <t>Shandong Taishan</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>5.38</v>
+        <v>3.88</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>15/04/2023 16:18</t>
+          <t>14/04/2023 13:16</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>7.05</v>
+        <v>3.16</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>16/04/2023 13:34</t>
+          <t>16/04/2023 13:30</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>3.66</v>
+        <v>3.42</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>15/04/2023 16:18</t>
+          <t>14/04/2023 13:16</t>
         </is>
       </c>
       <c r="P9" t="n">
-        <v>4.04</v>
+        <v>3.31</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>16/04/2023 13:34</t>
+          <t>16/04/2023 13:27</t>
         </is>
       </c>
       <c r="R9" t="n">
-        <v>1.67</v>
+        <v>1.98</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>15/04/2023 16:18</t>
+          <t>14/04/2023 13:16</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>1.51</v>
+        <v>2.35</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>16/04/2023 13:34</t>
+          <t>16/04/2023 13:30</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/shenzhen-fc-qingdao-hainiu/YcCyH7oh/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/shanghai-shenhua-shandong-taishan/4O7XHmWo/</t>
         </is>
       </c>
     </row>
@@ -7657,71 +7657,71 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Shenzhen</t>
+          <t>Shanghai Shenhua</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Meizhou Hakka</t>
+          <t>Henan Songshan Longmen</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J79" t="n">
-        <v>3.92</v>
+        <v>1.56</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>24/05/2023 13:42</t>
+          <t>26/05/2023 16:42</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>3.04</v>
+        <v>1.51</v>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>28/05/2023 13:33</t>
+          <t>28/05/2023 12:50</t>
         </is>
       </c>
       <c r="N79" t="n">
-        <v>3.58</v>
+        <v>4.2</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>24/05/2023 13:42</t>
+          <t>26/05/2023 16:42</t>
         </is>
       </c>
       <c r="P79" t="n">
-        <v>3.08</v>
+        <v>4.15</v>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>28/05/2023 13:33</t>
+          <t>28/05/2023 13:02</t>
         </is>
       </c>
       <c r="R79" t="n">
-        <v>1.94</v>
+        <v>5.85</v>
       </c>
       <c r="S79" t="inlineStr">
         <is>
-          <t>24/05/2023 13:42</t>
+          <t>26/05/2023 16:42</t>
         </is>
       </c>
       <c r="T79" t="n">
-        <v>2.57</v>
+        <v>6.91</v>
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>28/05/2023 13:33</t>
+          <t>28/05/2023 13:02</t>
         </is>
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/shenzhen-fc-meizhou-hakka/Qs6kUWra/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/shanghai-shenhua-henan-songshan-longmen/rJGpVCTh/</t>
         </is>
       </c>
     </row>
@@ -7749,71 +7749,71 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Shanghai Shenhua</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Henan Songshan Longmen</t>
+          <t>Meizhou Hakka</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J80" t="n">
-        <v>1.56</v>
+        <v>3.92</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>26/05/2023 16:42</t>
+          <t>24/05/2023 13:42</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>1.51</v>
+        <v>3.04</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>28/05/2023 12:50</t>
+          <t>28/05/2023 13:33</t>
         </is>
       </c>
       <c r="N80" t="n">
-        <v>4.2</v>
+        <v>3.58</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>26/05/2023 16:42</t>
+          <t>24/05/2023 13:42</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>4.15</v>
+        <v>3.08</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>28/05/2023 13:02</t>
+          <t>28/05/2023 13:33</t>
         </is>
       </c>
       <c r="R80" t="n">
-        <v>5.85</v>
+        <v>1.94</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>26/05/2023 16:42</t>
+          <t>24/05/2023 13:42</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>6.91</v>
+        <v>2.57</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>28/05/2023 13:02</t>
+          <t>28/05/2023 13:33</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/shanghai-shenhua-henan-songshan-longmen/rJGpVCTh/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/shenzhen-fc-meizhou-hakka/Qs6kUWra/</t>
         </is>
       </c>
     </row>
@@ -7933,46 +7933,46 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Beijing Guoan</t>
+          <t>Zhejiang Professional</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Changchun Yatai</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>1.57</v>
+        <v>1.32</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>29/05/2023 13:41</t>
+          <t>28/05/2023 13:42</t>
         </is>
       </c>
       <c r="L82" t="n">
-        <v>1.56</v>
+        <v>1.68</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>02/06/2023 13:29</t>
+          <t>02/06/2023 13:34</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>4.27</v>
+        <v>4.96</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>29/05/2023 13:41</t>
+          <t>28/05/2023 13:42</t>
         </is>
       </c>
       <c r="P82" t="n">
-        <v>4.37</v>
+        <v>4.15</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
@@ -7980,15 +7980,15 @@
         </is>
       </c>
       <c r="R82" t="n">
-        <v>5.97</v>
+        <v>8.08</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
-          <t>29/05/2023 13:41</t>
+          <t>28/05/2023 13:42</t>
         </is>
       </c>
       <c r="T82" t="n">
-        <v>5.49</v>
+        <v>4.73</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
@@ -7997,7 +7997,7 @@
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/beijing-guoan-changchun-yatai/Y79cSADB/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/zhejiang-professional-shenzhen-fc/Cb81RUSH/</t>
         </is>
       </c>
     </row>
@@ -8025,71 +8025,71 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Zhejiang Professional</t>
+          <t>Beijing Guoan</t>
         </is>
       </c>
       <c r="G83" t="n">
+        <v>4</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Changchun Yatai</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
         <v>3</v>
       </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Shenzhen</t>
-        </is>
-      </c>
-      <c r="I83" t="n">
-        <v>0</v>
-      </c>
       <c r="J83" t="n">
-        <v>1.32</v>
+        <v>1.57</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>28/05/2023 13:42</t>
+          <t>29/05/2023 13:41</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>1.68</v>
+        <v>1.56</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
+          <t>02/06/2023 13:29</t>
+        </is>
+      </c>
+      <c r="N83" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>29/05/2023 13:41</t>
+        </is>
+      </c>
+      <c r="P83" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
           <t>02/06/2023 13:34</t>
         </is>
       </c>
-      <c r="N83" t="n">
-        <v>4.96</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>28/05/2023 13:42</t>
-        </is>
-      </c>
-      <c r="P83" t="n">
-        <v>4.15</v>
-      </c>
-      <c r="Q83" t="inlineStr">
+      <c r="R83" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>29/05/2023 13:41</t>
+        </is>
+      </c>
+      <c r="T83" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="U83" t="inlineStr">
         <is>
           <t>02/06/2023 13:34</t>
         </is>
       </c>
-      <c r="R83" t="n">
-        <v>8.08</v>
-      </c>
-      <c r="S83" t="inlineStr">
-        <is>
-          <t>28/05/2023 13:42</t>
-        </is>
-      </c>
-      <c r="T83" t="n">
-        <v>4.73</v>
-      </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>02/06/2023 13:34</t>
-        </is>
-      </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/zhejiang-professional-shenzhen-fc/Cb81RUSH/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/beijing-guoan-changchun-yatai/Y79cSADB/</t>
         </is>
       </c>
     </row>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Qingdao Hainiu</t>
+          <t>Chengdu Rongcheng</t>
         </is>
       </c>
       <c r="G91" t="n">
@@ -8769,63 +8769,63 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Shanghai Shenhua</t>
+          <t>Tianjin Jinmen Tiger</t>
         </is>
       </c>
       <c r="I91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J91" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>04/06/2023 09:42</t>
+        </is>
+      </c>
+      <c r="L91" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>08/06/2023 13:17</t>
+        </is>
+      </c>
+      <c r="N91" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>04/06/2023 09:42</t>
+        </is>
+      </c>
+      <c r="P91" t="n">
         <v>3.57</v>
       </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>04/06/2023 11:42</t>
-        </is>
-      </c>
-      <c r="L91" t="n">
-        <v>4.16</v>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>08/06/2023 13:34</t>
-        </is>
-      </c>
-      <c r="N91" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>04/06/2023 11:42</t>
-        </is>
-      </c>
-      <c r="P91" t="n">
-        <v>3.26</v>
-      </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>08/06/2023 13:34</t>
+          <t>08/06/2023 13:17</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>2.18</v>
+        <v>6.45</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
-          <t>04/06/2023 11:42</t>
+          <t>04/06/2023 09:42</t>
         </is>
       </c>
       <c r="T91" t="n">
-        <v>2.01</v>
+        <v>5.24</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>08/06/2023 13:34</t>
+          <t>08/06/2023 13:17</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/qingdao-hainiu-shanghai-shenhua/8pMZR1JS/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/chengdu-rongcheng-tianjin-jinmen-tiger/QLWUSs4M/</t>
         </is>
       </c>
     </row>
@@ -8853,7 +8853,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Chengdu Rongcheng</t>
+          <t>Qingdao Hainiu</t>
         </is>
       </c>
       <c r="G92" t="n">
@@ -8861,63 +8861,63 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Tianjin Jinmen Tiger</t>
+          <t>Shanghai Shenhua</t>
         </is>
       </c>
       <c r="I92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J92" t="n">
-        <v>1.56</v>
+        <v>3.57</v>
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>04/06/2023 09:42</t>
+          <t>04/06/2023 11:42</t>
         </is>
       </c>
       <c r="L92" t="n">
-        <v>1.74</v>
+        <v>4.16</v>
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>08/06/2023 13:17</t>
+          <t>08/06/2023 13:34</t>
         </is>
       </c>
       <c r="N92" t="n">
-        <v>3.9</v>
+        <v>3.39</v>
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>04/06/2023 09:42</t>
+          <t>04/06/2023 11:42</t>
         </is>
       </c>
       <c r="P92" t="n">
-        <v>3.57</v>
+        <v>3.26</v>
       </c>
       <c r="Q92" t="inlineStr">
         <is>
-          <t>08/06/2023 13:17</t>
+          <t>08/06/2023 13:34</t>
         </is>
       </c>
       <c r="R92" t="n">
-        <v>6.45</v>
+        <v>2.18</v>
       </c>
       <c r="S92" t="inlineStr">
         <is>
-          <t>04/06/2023 09:42</t>
+          <t>04/06/2023 11:42</t>
         </is>
       </c>
       <c r="T92" t="n">
-        <v>5.24</v>
+        <v>2.01</v>
       </c>
       <c r="U92" t="inlineStr">
         <is>
-          <t>08/06/2023 13:17</t>
+          <t>08/06/2023 13:34</t>
         </is>
       </c>
       <c r="V92" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/chengdu-rongcheng-tianjin-jinmen-tiger/QLWUSs4M/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/qingdao-hainiu-shanghai-shenhua/8pMZR1JS/</t>
         </is>
       </c>
     </row>
@@ -9405,22 +9405,22 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Zhejiang Professional</t>
+          <t>Wuhan Three Towns</t>
         </is>
       </c>
       <c r="G98" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Meizhou Hakka</t>
+          <t>Dalian Pro</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>1.72</v>
+        <v>1.3</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>2</v>
+        <v>1.31</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="N98" t="n">
-        <v>3.85</v>
+        <v>5.49</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,15 +9444,15 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>3.67</v>
+        <v>5.58</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
-          <t>28/06/2023 13:33</t>
+          <t>28/06/2023 13:34</t>
         </is>
       </c>
       <c r="R98" t="n">
-        <v>4.76</v>
+        <v>7.51</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,16 +9460,16 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>3.65</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
-          <t>28/06/2023 13:33</t>
+          <t>28/06/2023 13:34</t>
         </is>
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/zhejiang-professional-meizhou-hakka/IXnvyudq/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/wuhan-three-towns-dalian-professional/nk0CuLmS/</t>
         </is>
       </c>
     </row>
@@ -9497,22 +9497,22 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Wuhan Three Towns</t>
+          <t>Tianjin Jinmen Tiger</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Dalian Pro</t>
+          <t>Qingdao Hainiu</t>
         </is>
       </c>
       <c r="I99" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J99" t="n">
-        <v>1.3</v>
+        <v>1.98</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>1.31</v>
+        <v>1.92</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
@@ -9528,7 +9528,7 @@
         </is>
       </c>
       <c r="N99" t="n">
-        <v>5.49</v>
+        <v>3.31</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,15 +9536,15 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>5.58</v>
+        <v>3.36</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>28/06/2023 13:34</t>
+          <t>28/06/2023 13:33</t>
         </is>
       </c>
       <c r="R99" t="n">
-        <v>7.51</v>
+        <v>4.16</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,16 +9552,16 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>9.199999999999999</v>
+        <v>4.42</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>28/06/2023 13:34</t>
+          <t>28/06/2023 13:33</t>
         </is>
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/wuhan-three-towns-dalian-professional/nk0CuLmS/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/tianjin-jinmen-tiger-qingdao-hainiu/8b18t1YL/</t>
         </is>
       </c>
     </row>
@@ -9589,22 +9589,22 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Tianjin Jinmen Tiger</t>
+          <t>Shanghai Shenhua</t>
         </is>
       </c>
       <c r="G100" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Qingdao Hainiu</t>
+          <t>Nantong Zhiyun</t>
         </is>
       </c>
       <c r="I100" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J100" t="n">
-        <v>1.98</v>
+        <v>1.56</v>
       </c>
       <c r="K100" t="inlineStr">
         <is>
@@ -9612,15 +9612,15 @@
         </is>
       </c>
       <c r="L100" t="n">
-        <v>1.92</v>
+        <v>1.6</v>
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>28/06/2023 13:33</t>
+          <t>28/06/2023 13:31</t>
         </is>
       </c>
       <c r="N100" t="n">
-        <v>3.31</v>
+        <v>3.82</v>
       </c>
       <c r="O100" t="inlineStr">
         <is>
@@ -9628,15 +9628,15 @@
         </is>
       </c>
       <c r="P100" t="n">
-        <v>3.36</v>
+        <v>3.57</v>
       </c>
       <c r="Q100" t="inlineStr">
         <is>
-          <t>28/06/2023 13:33</t>
+          <t>28/06/2023 13:32</t>
         </is>
       </c>
       <c r="R100" t="n">
-        <v>4.16</v>
+        <v>6.79</v>
       </c>
       <c r="S100" t="inlineStr">
         <is>
@@ -9644,16 +9644,16 @@
         </is>
       </c>
       <c r="T100" t="n">
-        <v>4.42</v>
+        <v>6.86</v>
       </c>
       <c r="U100" t="inlineStr">
         <is>
-          <t>28/06/2023 13:33</t>
+          <t>28/06/2023 13:32</t>
         </is>
       </c>
       <c r="V100" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/tianjin-jinmen-tiger-qingdao-hainiu/8b18t1YL/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/shanghai-shenhua-nantong-zhiyun/CW7arN39/</t>
         </is>
       </c>
     </row>
@@ -9681,22 +9681,22 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Shanghai Shenhua</t>
+          <t>Cangzhou</t>
         </is>
       </c>
       <c r="G101" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Henan Songshan Longmen</t>
+        </is>
+      </c>
+      <c r="I101" t="n">
         <v>1</v>
       </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>Nantong Zhiyun</t>
-        </is>
-      </c>
-      <c r="I101" t="n">
-        <v>0</v>
-      </c>
       <c r="J101" t="n">
-        <v>1.56</v>
+        <v>2.14</v>
       </c>
       <c r="K101" t="inlineStr">
         <is>
@@ -9704,15 +9704,15 @@
         </is>
       </c>
       <c r="L101" t="n">
-        <v>1.6</v>
+        <v>2.48</v>
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>28/06/2023 13:31</t>
+          <t>28/06/2023 13:34</t>
         </is>
       </c>
       <c r="N101" t="n">
-        <v>3.82</v>
+        <v>3.39</v>
       </c>
       <c r="O101" t="inlineStr">
         <is>
@@ -9720,15 +9720,15 @@
         </is>
       </c>
       <c r="P101" t="n">
-        <v>3.57</v>
+        <v>3.26</v>
       </c>
       <c r="Q101" t="inlineStr">
         <is>
-          <t>28/06/2023 13:32</t>
+          <t>28/06/2023 13:33</t>
         </is>
       </c>
       <c r="R101" t="n">
-        <v>6.79</v>
+        <v>3.24</v>
       </c>
       <c r="S101" t="inlineStr">
         <is>
@@ -9736,16 +9736,16 @@
         </is>
       </c>
       <c r="T101" t="n">
-        <v>6.86</v>
+        <v>2.99</v>
       </c>
       <c r="U101" t="inlineStr">
         <is>
-          <t>28/06/2023 13:32</t>
+          <t>28/06/2023 13:34</t>
         </is>
       </c>
       <c r="V101" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/shanghai-shenhua-nantong-zhiyun/CW7arN39/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/cangzhou-mighty-lions-henan-songshan-longmen/QZB3ssJF/</t>
         </is>
       </c>
     </row>
@@ -9773,22 +9773,22 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Cangzhou</t>
+          <t>Zhejiang Professional</t>
         </is>
       </c>
       <c r="G102" t="n">
+        <v>3</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Meizhou Hakka</t>
+        </is>
+      </c>
+      <c r="I102" t="n">
         <v>0</v>
       </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>Henan Songshan Longmen</t>
-        </is>
-      </c>
-      <c r="I102" t="n">
-        <v>1</v>
-      </c>
       <c r="J102" t="n">
-        <v>2.14</v>
+        <v>1.72</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
@@ -9796,15 +9796,15 @@
         </is>
       </c>
       <c r="L102" t="n">
-        <v>2.48</v>
+        <v>2</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>28/06/2023 13:34</t>
+          <t>28/06/2023 13:33</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>3.39</v>
+        <v>3.85</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -9812,7 +9812,7 @@
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.26</v>
+        <v>3.67</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
@@ -9820,7 +9820,7 @@
         </is>
       </c>
       <c r="R102" t="n">
-        <v>3.24</v>
+        <v>4.76</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
@@ -9828,16 +9828,16 @@
         </is>
       </c>
       <c r="T102" t="n">
-        <v>2.99</v>
+        <v>3.65</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>28/06/2023 13:34</t>
+          <t>28/06/2023 13:33</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/cangzhou-mighty-lions-henan-songshan-longmen/QZB3ssJF/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/zhejiang-professional-meizhou-hakka/IXnvyudq/</t>
         </is>
       </c>
     </row>
@@ -21181,71 +21181,71 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>Beijing Guoan</t>
+          <t>Zhejiang Professional</t>
         </is>
       </c>
       <c r="G226" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>Chengdu Rongcheng</t>
+          <t>Cangzhou</t>
         </is>
       </c>
       <c r="I226" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J226" t="n">
-        <v>2.5</v>
+        <v>1.44</v>
       </c>
       <c r="K226" t="inlineStr">
         <is>
-          <t>23/10/2023 13:42</t>
+          <t>22/10/2023 09:42</t>
         </is>
       </c>
       <c r="L226" t="n">
-        <v>2.75</v>
+        <v>1.15</v>
       </c>
       <c r="M226" t="inlineStr">
         <is>
+          <t>29/10/2023 08:05</t>
+        </is>
+      </c>
+      <c r="N226" t="n">
+        <v>4.73</v>
+      </c>
+      <c r="O226" t="inlineStr">
+        <is>
+          <t>22/10/2023 09:42</t>
+        </is>
+      </c>
+      <c r="P226" t="n">
+        <v>7.84</v>
+      </c>
+      <c r="Q226" t="inlineStr">
+        <is>
           <t>29/10/2023 08:29</t>
         </is>
       </c>
-      <c r="N226" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="O226" t="inlineStr">
-        <is>
-          <t>23/10/2023 13:42</t>
-        </is>
-      </c>
-      <c r="P226" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="Q226" t="inlineStr">
-        <is>
-          <t>29/10/2023 08:22</t>
-        </is>
-      </c>
       <c r="R226" t="n">
-        <v>2.93</v>
+        <v>6.87</v>
       </c>
       <c r="S226" t="inlineStr">
         <is>
-          <t>23/10/2023 13:42</t>
+          <t>22/10/2023 09:42</t>
         </is>
       </c>
       <c r="T226" t="n">
-        <v>2.68</v>
+        <v>13.88</v>
       </c>
       <c r="U226" t="inlineStr">
         <is>
-          <t>29/10/2023 08:22</t>
+          <t>29/10/2023 08:29</t>
         </is>
       </c>
       <c r="V226" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/beijing-guoan-chengdu-rongcheng/YX4RMOfF/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/zhejiang-professional-cangzhou-mighty-lions/YemEDKH1/</t>
         </is>
       </c>
     </row>
@@ -21273,7 +21273,7 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>Henan Songshan Longmen</t>
+          <t>Wuhan Three Towns</t>
         </is>
       </c>
       <c r="G227" t="n">
@@ -21281,63 +21281,63 @@
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>Changchun Yatai</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="I227" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J227" t="n">
-        <v>2.08</v>
+        <v>1.04</v>
       </c>
       <c r="K227" t="inlineStr">
         <is>
-          <t>22/10/2023 09:42</t>
+          <t>23/10/2023 13:42</t>
         </is>
       </c>
       <c r="L227" t="n">
-        <v>1.55</v>
+        <v>1.03</v>
       </c>
       <c r="M227" t="inlineStr">
         <is>
-          <t>29/10/2023 08:12</t>
+          <t>29/10/2023 08:27</t>
         </is>
       </c>
       <c r="N227" t="n">
-        <v>3.48</v>
+        <v>20.46</v>
       </c>
       <c r="O227" t="inlineStr">
         <is>
-          <t>22/10/2023 09:42</t>
+          <t>23/10/2023 13:42</t>
         </is>
       </c>
       <c r="P227" t="n">
-        <v>4.2</v>
+        <v>22.64</v>
       </c>
       <c r="Q227" t="inlineStr">
         <is>
-          <t>29/10/2023 08:12</t>
+          <t>29/10/2023 08:29</t>
         </is>
       </c>
       <c r="R227" t="n">
-        <v>3.59</v>
+        <v>45.47</v>
       </c>
       <c r="S227" t="inlineStr">
         <is>
-          <t>22/10/2023 09:42</t>
+          <t>23/10/2023 13:42</t>
         </is>
       </c>
       <c r="T227" t="n">
-        <v>5.58</v>
+        <v>42.44</v>
       </c>
       <c r="U227" t="inlineStr">
         <is>
-          <t>29/10/2023 08:12</t>
+          <t>29/10/2023 08:29</t>
         </is>
       </c>
       <c r="V227" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/henan-songshan-longmen-changchun-yatai/CO3VLrAL/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/wuhan-three-towns-shenzhen-fc/4MrAE02e/</t>
         </is>
       </c>
     </row>
@@ -21365,22 +21365,22 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Meizhou Hakka</t>
+          <t>Tianjin Jinmen Tiger</t>
         </is>
       </c>
       <c r="G228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>Nantong Zhiyun</t>
+          <t>Shanghai Shenhua</t>
         </is>
       </c>
       <c r="I228" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J228" t="n">
-        <v>1.75</v>
+        <v>2.66</v>
       </c>
       <c r="K228" t="inlineStr">
         <is>
@@ -21388,7 +21388,7 @@
         </is>
       </c>
       <c r="L228" t="n">
-        <v>1.65</v>
+        <v>3.31</v>
       </c>
       <c r="M228" t="inlineStr">
         <is>
@@ -21396,7 +21396,7 @@
         </is>
       </c>
       <c r="N228" t="n">
-        <v>3.86</v>
+        <v>3.06</v>
       </c>
       <c r="O228" t="inlineStr">
         <is>
@@ -21404,32 +21404,32 @@
         </is>
       </c>
       <c r="P228" t="n">
-        <v>4.26</v>
+        <v>3.14</v>
       </c>
       <c r="Q228" t="inlineStr">
         <is>
+          <t>29/10/2023 07:42</t>
+        </is>
+      </c>
+      <c r="R228" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="S228" t="inlineStr">
+        <is>
+          <t>22/10/2023 09:42</t>
+        </is>
+      </c>
+      <c r="T228" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="U228" t="inlineStr">
+        <is>
           <t>29/10/2023 08:29</t>
         </is>
       </c>
-      <c r="R228" t="n">
-        <v>4.07</v>
-      </c>
-      <c r="S228" t="inlineStr">
-        <is>
-          <t>22/10/2023 09:42</t>
-        </is>
-      </c>
-      <c r="T228" t="n">
-        <v>4.79</v>
-      </c>
-      <c r="U228" t="inlineStr">
-        <is>
-          <t>29/10/2023 08:29</t>
-        </is>
-      </c>
       <c r="V228" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/meizhou-hakka-nantong-zhiyun/6BYUN4u9/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/tianjin-jinmen-tiger-shanghai-shenhua/QVq6Ftmk/</t>
         </is>
       </c>
     </row>
@@ -21457,22 +21457,22 @@
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>Qingdao Hainiu</t>
+          <t>Shanghai Port</t>
         </is>
       </c>
       <c r="G229" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>Dalian Pro</t>
+          <t>Shandong Taishan</t>
         </is>
       </c>
       <c r="I229" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J229" t="n">
-        <v>1.91</v>
+        <v>2.27</v>
       </c>
       <c r="K229" t="inlineStr">
         <is>
@@ -21480,15 +21480,15 @@
         </is>
       </c>
       <c r="L229" t="n">
-        <v>2.97</v>
+        <v>2.43</v>
       </c>
       <c r="M229" t="inlineStr">
         <is>
-          <t>29/10/2023 08:18</t>
+          <t>29/10/2023 08:24</t>
         </is>
       </c>
       <c r="N229" t="n">
-        <v>3.62</v>
+        <v>3.38</v>
       </c>
       <c r="O229" t="inlineStr">
         <is>
@@ -21496,15 +21496,15 @@
         </is>
       </c>
       <c r="P229" t="n">
-        <v>3.59</v>
+        <v>3.47</v>
       </c>
       <c r="Q229" t="inlineStr">
         <is>
-          <t>29/10/2023 08:17</t>
+          <t>29/10/2023 08:29</t>
         </is>
       </c>
       <c r="R229" t="n">
-        <v>3.66</v>
+        <v>3.21</v>
       </c>
       <c r="S229" t="inlineStr">
         <is>
@@ -21512,16 +21512,16 @@
         </is>
       </c>
       <c r="T229" t="n">
-        <v>2.27</v>
+        <v>2.9</v>
       </c>
       <c r="U229" t="inlineStr">
         <is>
-          <t>29/10/2023 08:18</t>
+          <t>29/10/2023 08:24</t>
         </is>
       </c>
       <c r="V229" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/qingdao-hainiu-dalian-professional/6o3ZK2PR/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/shanghai-port-shandong-taishan/r7f1GMXr/</t>
         </is>
       </c>
     </row>
@@ -21549,22 +21549,22 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>Shanghai Port</t>
+          <t>Meizhou Hakka</t>
         </is>
       </c>
       <c r="G230" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>Shandong Taishan</t>
+          <t>Nantong Zhiyun</t>
         </is>
       </c>
       <c r="I230" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J230" t="n">
-        <v>2.27</v>
+        <v>1.75</v>
       </c>
       <c r="K230" t="inlineStr">
         <is>
@@ -21572,15 +21572,15 @@
         </is>
       </c>
       <c r="L230" t="n">
-        <v>2.43</v>
+        <v>1.65</v>
       </c>
       <c r="M230" t="inlineStr">
         <is>
-          <t>29/10/2023 08:24</t>
+          <t>29/10/2023 08:29</t>
         </is>
       </c>
       <c r="N230" t="n">
-        <v>3.38</v>
+        <v>3.86</v>
       </c>
       <c r="O230" t="inlineStr">
         <is>
@@ -21588,7 +21588,7 @@
         </is>
       </c>
       <c r="P230" t="n">
-        <v>3.47</v>
+        <v>4.26</v>
       </c>
       <c r="Q230" t="inlineStr">
         <is>
@@ -21596,7 +21596,7 @@
         </is>
       </c>
       <c r="R230" t="n">
-        <v>3.21</v>
+        <v>4.07</v>
       </c>
       <c r="S230" t="inlineStr">
         <is>
@@ -21604,16 +21604,16 @@
         </is>
       </c>
       <c r="T230" t="n">
-        <v>2.9</v>
+        <v>4.79</v>
       </c>
       <c r="U230" t="inlineStr">
         <is>
-          <t>29/10/2023 08:24</t>
+          <t>29/10/2023 08:29</t>
         </is>
       </c>
       <c r="V230" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/shanghai-port-shandong-taishan/r7f1GMXr/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/meizhou-hakka-nantong-zhiyun/6BYUN4u9/</t>
         </is>
       </c>
     </row>
@@ -21641,7 +21641,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>Tianjin Jinmen Tiger</t>
+          <t>Henan Songshan Longmen</t>
         </is>
       </c>
       <c r="G231" t="n">
@@ -21649,14 +21649,14 @@
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>Shanghai Shenhua</t>
+          <t>Changchun Yatai</t>
         </is>
       </c>
       <c r="I231" t="n">
         <v>1</v>
       </c>
       <c r="J231" t="n">
-        <v>2.66</v>
+        <v>2.08</v>
       </c>
       <c r="K231" t="inlineStr">
         <is>
@@ -21664,15 +21664,15 @@
         </is>
       </c>
       <c r="L231" t="n">
-        <v>3.31</v>
+        <v>1.55</v>
       </c>
       <c r="M231" t="inlineStr">
         <is>
-          <t>29/10/2023 08:29</t>
+          <t>29/10/2023 08:12</t>
         </is>
       </c>
       <c r="N231" t="n">
-        <v>3.06</v>
+        <v>3.48</v>
       </c>
       <c r="O231" t="inlineStr">
         <is>
@@ -21680,15 +21680,15 @@
         </is>
       </c>
       <c r="P231" t="n">
-        <v>3.14</v>
+        <v>4.2</v>
       </c>
       <c r="Q231" t="inlineStr">
         <is>
-          <t>29/10/2023 07:42</t>
+          <t>29/10/2023 08:12</t>
         </is>
       </c>
       <c r="R231" t="n">
-        <v>2.9</v>
+        <v>3.59</v>
       </c>
       <c r="S231" t="inlineStr">
         <is>
@@ -21696,16 +21696,16 @@
         </is>
       </c>
       <c r="T231" t="n">
-        <v>2.36</v>
+        <v>5.58</v>
       </c>
       <c r="U231" t="inlineStr">
         <is>
-          <t>29/10/2023 08:29</t>
+          <t>29/10/2023 08:12</t>
         </is>
       </c>
       <c r="V231" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/tianjin-jinmen-tiger-shanghai-shenhua/QVq6Ftmk/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/henan-songshan-longmen-changchun-yatai/CO3VLrAL/</t>
         </is>
       </c>
     </row>
@@ -21733,22 +21733,22 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>Wuhan Three Towns</t>
+          <t>Beijing Guoan</t>
         </is>
       </c>
       <c r="G232" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>Shenzhen</t>
+          <t>Chengdu Rongcheng</t>
         </is>
       </c>
       <c r="I232" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J232" t="n">
-        <v>1.04</v>
+        <v>2.5</v>
       </c>
       <c r="K232" t="inlineStr">
         <is>
@@ -21756,15 +21756,15 @@
         </is>
       </c>
       <c r="L232" t="n">
-        <v>1.03</v>
+        <v>2.75</v>
       </c>
       <c r="M232" t="inlineStr">
         <is>
-          <t>29/10/2023 08:27</t>
+          <t>29/10/2023 08:29</t>
         </is>
       </c>
       <c r="N232" t="n">
-        <v>20.46</v>
+        <v>3.27</v>
       </c>
       <c r="O232" t="inlineStr">
         <is>
@@ -21772,15 +21772,15 @@
         </is>
       </c>
       <c r="P232" t="n">
-        <v>22.64</v>
+        <v>3.27</v>
       </c>
       <c r="Q232" t="inlineStr">
         <is>
-          <t>29/10/2023 08:29</t>
+          <t>29/10/2023 08:22</t>
         </is>
       </c>
       <c r="R232" t="n">
-        <v>45.47</v>
+        <v>2.93</v>
       </c>
       <c r="S232" t="inlineStr">
         <is>
@@ -21788,16 +21788,16 @@
         </is>
       </c>
       <c r="T232" t="n">
-        <v>42.44</v>
+        <v>2.68</v>
       </c>
       <c r="U232" t="inlineStr">
         <is>
-          <t>29/10/2023 08:29</t>
+          <t>29/10/2023 08:22</t>
         </is>
       </c>
       <c r="V232" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/china/super-league/wuhan-three-towns-shenzhen-fc/4MrAE02e/</t>
+          <t>https://www.betexplorer.com/football/china/super-league/beijing-guoan-chengdu-rongcheng/YX4RMOfF/</t>
         </is>
       </c>
     </row>
@@ -21825,71 +21825,715 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
+          <t>Qingdao Hainiu</t>
+        </is>
+      </c>
+      <c r="G233" t="n">
+        <v>2</v>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>Dalian Pro</t>
+        </is>
+      </c>
+      <c r="I233" t="n">
+        <v>2</v>
+      </c>
+      <c r="J233" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>22/10/2023 09:42</t>
+        </is>
+      </c>
+      <c r="L233" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="M233" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:18</t>
+        </is>
+      </c>
+      <c r="N233" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="O233" t="inlineStr">
+        <is>
+          <t>22/10/2023 09:42</t>
+        </is>
+      </c>
+      <c r="P233" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="Q233" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:17</t>
+        </is>
+      </c>
+      <c r="R233" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="S233" t="inlineStr">
+        <is>
+          <t>22/10/2023 09:42</t>
+        </is>
+      </c>
+      <c r="T233" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="U233" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:18</t>
+        </is>
+      </c>
+      <c r="V233" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/china/super-league/qingdao-hainiu-dalian-professional/6o3ZK2PR/</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>china</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>super-league</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E234" s="2" t="n">
+        <v>45234.35416666666</v>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>Shandong Taishan</t>
+        </is>
+      </c>
+      <c r="G234" t="n">
+        <v>5</v>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>Henan Songshan Longmen</t>
+        </is>
+      </c>
+      <c r="I234" t="n">
+        <v>1</v>
+      </c>
+      <c r="J234" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="K234" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="L234" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="M234" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="N234" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="O234" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="P234" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="Q234" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="R234" t="n">
+        <v>9.880000000000001</v>
+      </c>
+      <c r="S234" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="T234" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="U234" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="V234" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/china/super-league/shandong-taishan-henan-songshan-longmen/buSCYLgR/</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>china</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>super-league</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E235" s="2" t="n">
+        <v>45234.35416666666</v>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>Cangzhou</t>
+        </is>
+      </c>
+      <c r="G235" t="n">
+        <v>0</v>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>Qingdao Hainiu</t>
+        </is>
+      </c>
+      <c r="I235" t="n">
+        <v>0</v>
+      </c>
+      <c r="J235" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:41</t>
+        </is>
+      </c>
+      <c r="L235" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="M235" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="N235" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="O235" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:41</t>
+        </is>
+      </c>
+      <c r="P235" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="Q235" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:27</t>
+        </is>
+      </c>
+      <c r="R235" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="S235" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:41</t>
+        </is>
+      </c>
+      <c r="T235" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="U235" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="V235" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/china/super-league/cangzhou-mighty-lions-qingdao-hainiu/CnnICvX7/</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>china</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>super-league</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E236" s="2" t="n">
+        <v>45234.35416666666</v>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>Changchun Yatai</t>
+        </is>
+      </c>
+      <c r="G236" t="n">
+        <v>3</v>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>Wuhan Three Towns</t>
+        </is>
+      </c>
+      <c r="I236" t="n">
+        <v>4</v>
+      </c>
+      <c r="J236" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="K236" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="L236" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="M236" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="N236" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="O236" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="P236" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="Q236" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="R236" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="S236" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="T236" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="U236" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="V236" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/china/super-league/changchun-yatai-wuhan-three-towns/EiQ0yO98/</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>china</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>super-league</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E237" s="2" t="n">
+        <v>45234.35416666666</v>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>Chengdu Rongcheng</t>
+        </is>
+      </c>
+      <c r="G237" t="n">
+        <v>3</v>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>Meizhou Hakka</t>
+        </is>
+      </c>
+      <c r="I237" t="n">
+        <v>0</v>
+      </c>
+      <c r="J237" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="K237" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="L237" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="M237" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:26</t>
+        </is>
+      </c>
+      <c r="N237" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="O237" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="P237" t="n">
+        <v>9.41</v>
+      </c>
+      <c r="Q237" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="R237" t="n">
+        <v>6.37</v>
+      </c>
+      <c r="S237" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="T237" t="n">
+        <v>16.26</v>
+      </c>
+      <c r="U237" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="V237" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/china/super-league/chengdu-rongcheng-meizhou-hakka/QRT4zrPE/</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>china</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>super-league</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E238" s="2" t="n">
+        <v>45234.35416666666</v>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>Dalian Pro</t>
+        </is>
+      </c>
+      <c r="G238" t="n">
+        <v>2</v>
+      </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>Shanghai Port</t>
+        </is>
+      </c>
+      <c r="I238" t="n">
+        <v>3</v>
+      </c>
+      <c r="J238" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="K238" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="L238" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="M238" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="N238" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="O238" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="P238" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="Q238" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="R238" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="S238" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="T238" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="U238" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="V238" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/china/super-league/dalian-professional-shanghai-port/KlT8Z1vL/</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>china</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>super-league</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E239" s="2" t="n">
+        <v>45234.35416666666</v>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>Nantong Zhiyun</t>
+        </is>
+      </c>
+      <c r="G239" t="n">
+        <v>1</v>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>Tianjin Jinmen Tiger</t>
+        </is>
+      </c>
+      <c r="I239" t="n">
+        <v>2</v>
+      </c>
+      <c r="J239" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="K239" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="L239" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="M239" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:27</t>
+        </is>
+      </c>
+      <c r="N239" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="O239" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="P239" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="Q239" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:17</t>
+        </is>
+      </c>
+      <c r="R239" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="S239" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="T239" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="U239" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:27</t>
+        </is>
+      </c>
+      <c r="V239" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/china/super-league/nantong-zhiyun-tianjin-jinmen-tiger/Cn8mSJWf/</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>china</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>super-league</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E240" s="2" t="n">
+        <v>45234.35416666666</v>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>Shanghai Shenhua</t>
+        </is>
+      </c>
+      <c r="G240" t="n">
+        <v>1</v>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
           <t>Zhejiang Professional</t>
         </is>
       </c>
-      <c r="G233" t="n">
-        <v>6</v>
-      </c>
-      <c r="H233" t="inlineStr">
-        <is>
-          <t>Cangzhou</t>
-        </is>
-      </c>
-      <c r="I233" t="n">
-        <v>1</v>
-      </c>
-      <c r="J233" t="n">
-        <v>1.44</v>
-      </c>
-      <c r="K233" t="inlineStr">
-        <is>
-          <t>22/10/2023 09:42</t>
-        </is>
-      </c>
-      <c r="L233" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="M233" t="inlineStr">
-        <is>
-          <t>29/10/2023 08:05</t>
-        </is>
-      </c>
-      <c r="N233" t="n">
-        <v>4.73</v>
-      </c>
-      <c r="O233" t="inlineStr">
-        <is>
-          <t>22/10/2023 09:42</t>
-        </is>
-      </c>
-      <c r="P233" t="n">
-        <v>7.84</v>
-      </c>
-      <c r="Q233" t="inlineStr">
-        <is>
-          <t>29/10/2023 08:29</t>
-        </is>
-      </c>
-      <c r="R233" t="n">
-        <v>6.87</v>
-      </c>
-      <c r="S233" t="inlineStr">
-        <is>
-          <t>22/10/2023 09:42</t>
-        </is>
-      </c>
-      <c r="T233" t="n">
-        <v>13.88</v>
-      </c>
-      <c r="U233" t="inlineStr">
-        <is>
-          <t>29/10/2023 08:29</t>
-        </is>
-      </c>
-      <c r="V233" t="inlineStr">
-        <is>
-          <t>https://www.betexplorer.com/football/china/super-league/zhejiang-professional-cangzhou-mighty-lions/YemEDKH1/</t>
+      <c r="I240" t="n">
+        <v>2</v>
+      </c>
+      <c r="J240" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K240" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="L240" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="M240" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="N240" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="O240" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="P240" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="Q240" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:26</t>
+        </is>
+      </c>
+      <c r="R240" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="S240" t="inlineStr">
+        <is>
+          <t>29/10/2023 08:42</t>
+        </is>
+      </c>
+      <c r="T240" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="U240" t="inlineStr">
+        <is>
+          <t>04/11/2023 08:29</t>
+        </is>
+      </c>
+      <c r="V240" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/china/super-league/shanghai-shenhua-zhejiang-professional/vZ9uUu2r/</t>
         </is>
       </c>
     </row>

</xml_diff>